<commit_message>
Employee Type in employee import template same as bound Property of model class
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\accupay\AccuPay\ImportTemplates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F972270-AF5B-40BE-9690-39932FFF1F63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="6210" tabRatio="397"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="6210" tabRatio="397" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Employees!$T$1:$T$1</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -76,9 +85,6 @@
     <t>Employment status(Probationary/Regular/Resigned/Terminated)</t>
   </si>
   <si>
-    <t>Employee Type(Weekly/Monthly)</t>
-  </si>
-  <si>
     <t>Pay frequency(Weekly/Semi-monthly)</t>
   </si>
   <si>
@@ -86,19 +92,22 @@
   </si>
   <si>
     <t>Works days per year</t>
+  </si>
+  <si>
+    <t>Employee Type(Daily/Monthly/Fixed)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
     <numFmt numFmtId="165" formatCode="000\-000\-000\-000"/>
     <numFmt numFmtId="166" formatCode="00\-0000000\-00"/>
     <numFmt numFmtId="167" formatCode="0000\-0000\-0000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -163,17 +172,21 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="0"/>
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -222,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,9 +267,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,6 +319,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -463,17 +512,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
@@ -494,14 +543,14 @@
     <col min="17" max="17" width="18.28515625" style="6" customWidth="1"/>
     <col min="18" max="18" width="28" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="32" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="60.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -527,7 +576,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>5</v>
@@ -557,10 +606,10 @@
         <v>18</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>19</v>
@@ -572,23 +621,23 @@
         <v>16</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="CD03" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="YvHqPBSk7MML83LC3A0McIIkT5XnzEcL91xUmWvBpJo5rIetsg3S5tfo0bshm7aJeZk9PIkgoZjXBtn/BgVsdw==" saltValue="NiJx0QHM30H8ib/o84tujg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Male,Female"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Single,Married"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S1:S1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"WEEKLY,SEMI-MONTHLY"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T1048576">
-      <formula1>"Daily,Monthly"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>"Daily,Monthly,Fixed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: remove weekly pay frequency options in employee and paystub form
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Employees" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Employees!$T$1:$T$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Employees!$S$1:$S$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Employee ID</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">Date employed(MM/dd/yyyy)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pay frequency(Weekly/Semi-monthly)</t>
   </si>
   <si>
     <t xml:space="preserve">Employee Type(Daily/Monthly/Fixed)</t>
@@ -180,7 +177,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,10 +223,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -264,13 +257,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="Z10" activeCellId="0" sqref="Z10"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="T18" activeCellId="0" sqref="T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.99"/>
@@ -290,15 +283,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="5" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="5" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="27.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="36.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="60.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="6" width="23.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="23" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="60.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="19.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="23" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -350,7 +343,7 @@
       <c r="Q1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="8" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="7" t="s">
@@ -359,19 +352,17 @@
       <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="12" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="14" t="s">
-        <v>22</v>
-      </c>
+      <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G1001" type="list">
       <formula1>"Male,Female"</formula1>
       <formula2>0</formula2>
@@ -381,10 +372,6 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S2:S1001" type="list">
-      <formula1>"WEEKLY,SEMI-MONTHLY"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T2:T1001" type="list">
       <formula1>"Daily,Monthly,Fixed"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
feat: save employee branch in import employee
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Employee ID</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">Works days per year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch</t>
   </si>
 </sst>
 </file>
@@ -97,7 +100,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
+    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="000\-000\-000\-000"/>
     <numFmt numFmtId="167" formatCode="00\-0000000\-00"/>
     <numFmt numFmtId="168" formatCode="0000\-0000\-0000"/>
@@ -257,13 +260,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="T18" activeCellId="0" sqref="T18"/>
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="bottomLeft" activeCell="W7" activeCellId="0" sqref="W7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.99"/>
@@ -287,8 +290,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="60.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="19.04"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="23" style="1" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="24" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,6 +361,9 @@
       </c>
       <c r="V1" s="13" t="s">
         <v>21</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>

</xml_diff>

<commit_message>
feat: save both vacation and sick leave allowance in import employee
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Employees" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Employees!$S$1:$S$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Employees!$R$1:$R$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -37,9 +37,6 @@
     <t xml:space="preserve">Middle name</t>
   </si>
   <si>
-    <t xml:space="preserve">Surname</t>
-  </si>
-  <si>
     <t xml:space="preserve">Birth date(MM/dd/yyyy)</t>
   </si>
   <si>
@@ -85,7 +82,10 @@
     <t xml:space="preserve">Employment status(Probationary/Regular/Resigned/Terminated)</t>
   </si>
   <si>
-    <t xml:space="preserve">Leave allowance per year</t>
+    <t xml:space="preserve">VL allowance per year (hours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SL allowance per year (hours)</t>
   </si>
   <si>
     <t xml:space="preserve">Works days per year</t>
@@ -138,12 +138,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBE33D"/>
+        <bgColor rgb="FFFFCC00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -180,7 +186,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -209,11 +215,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -229,7 +239,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -250,6 +268,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FFBBE33D"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -260,10 +338,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="W7" activeCellId="0" sqref="W7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="S15" activeCellId="0" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -272,30 +350,29 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="75.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="39.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="24.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="5" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="5" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="27.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="60.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="24" style="1" width="9.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="23.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="34.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="75.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="39.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="22.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="24.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="5" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="5" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="27.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="60.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="28.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="21.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="23" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -305,80 +382,81 @@
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="16" t="s">
         <v>22</v>
       </c>
+      <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G1001" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F2:F1001" type="list">
       <formula1>"Male,Female"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I2:I1001" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H1001" type="list">
       <formula1>"Single,Married"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S2:S1001" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R2:R1001" type="list">
       <formula1>"Daily,Monthly,Fixed"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
feat: save ATM number in import employee and improve other old forms
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Employee ID</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t xml:space="preserve">Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current VL balance (hours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current SL balance (hours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM No./Account No.</t>
   </si>
 </sst>
 </file>
@@ -231,8 +240,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -341,7 +350,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="S15" activeCellId="0" sqref="S15"/>
+      <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -368,7 +377,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="26.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="28.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="23" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="27" style="1" width="9.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -406,7 +419,7 @@
       <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="10" t="s">
@@ -439,8 +452,17 @@
       <c r="V1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="W1" s="15" t="s">
         <v>22</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>

</xml_diff>

<commit_message>
feat: add email, rest day and email in import template
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
@@ -22,8 +22,38 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="AB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Sunday
+Monday
+Tuesday
+Wednesday
+Thursday
+Friday
+Saturday</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Employee ID</t>
   </si>
@@ -101,6 +131,15 @@
   </si>
   <si>
     <t xml:space="preserve">ATM No./Account No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grace Period (mins.)</t>
   </si>
 </sst>
 </file>
@@ -347,10 +386,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
+      <selection pane="bottomLeft" activeCell="AB1" activeCellId="0" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -379,9 +418,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="26.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="21.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="27" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="31" style="1" width="9.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -463,6 +506,15 @@
       </c>
       <c r="Z1" s="16" t="s">
         <v>25</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -490,5 +542,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: addes support for Single parent leave feature
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-employeelist-template.xlsx
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lambert\accupay\AccuPay\ImportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Oeb4NL6TP9ZhtyxGysa10tvzjBSJoB7daVaeaIYqQxot4PKDha3QDofHTIBa4T3FYMMA+sL0GU+zbW/ghuCChw==" workbookSaltValue="3rpbjtZVmb2d6LR/lSd0vA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -24,36 +25,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="AB1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sunday
-Monday
-Tuesday
-Wednesday
-Thursday
-Friday
-Saturday</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -219,19 +190,37 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,6 +344,150 @@
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
           <a:headEnd/>
           <a:tailEnd/>
         </a:ln>
@@ -627,12 +760,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -667,73 +799,73 @@
     <col min="27" max="27" width="21.28515625" style="1" customWidth="1"/>
     <col min="28" max="28" width="17.5703125" style="1" customWidth="1"/>
     <col min="29" max="29" width="20.42578125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="17.5703125" style="1" customWidth="1"/>
-    <col min="31" max="1021" width="9.140625" style="1" customWidth="1"/>
-    <col min="1022" max="1025" width="11.5703125"/>
+    <col min="30" max="1020" width="9.140625" style="7" customWidth="1"/>
+    <col min="1021" max="1024" width="11.5703125" style="7"/>
+    <col min="1025" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="15" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="15" t="s">
@@ -760,12 +892,10 @@
       <c r="AC1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="AMH1"/>
-      <c r="AMI1"/>
-      <c r="AMJ1"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <sheetProtection algorithmName="SHA-512" hashValue="swB3sfZSnZ8Ht4mqV6naowgmdnumDDHVPhY1oYP9PxfXfoeXZzePF+E7D/q9NryitBaDfN8Xa2FAtF4by8CxrQ==" saltValue="iQUKtiubs+crd2hfKB1hGQ==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1001">
       <formula1>"Male,Female"</formula1>
       <formula2>0</formula2>
@@ -778,10 +908,23 @@
       <formula1>"Daily,Monthly,Fixed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB1048576">
+      <formula1>"Sunday,Monday,Tuesday,Wednesday,Thursday,Friday,Saturday"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC1048576">
+      <formula1>0</formula1>
+      <formula2>1440</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576">
+      <formula1>"Regular,Probationary,Resigned,Terminated"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:Y1048576 T2:U1048576 V2:V1048576">
+      <formula1>0</formula1>
+      <formula2>999.99</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>